<commit_message>
RulerLineInfo/Level, pixToTimeStamp, VRuler.js_lines impl
</commit_message>
<xml_diff>
--- a/purescript/misc/util.xlsx
+++ b/purescript/misc/util.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t xml:space="preserve">left</t>
   </si>
@@ -128,6 +128,21 @@
     <t xml:space="preserve">Padding</t>
   </si>
   <si>
+    <t xml:space="preserve">Start date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unix time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seconds pr day</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vruler</t>
   </si>
   <si>
@@ -147,14 +162,22 @@
   </si>
   <si>
     <t xml:space="preserve">sections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hruler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ppx (padding)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="MM/DD/YYYY\ HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="MM/DD/YY"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -300,7 +323,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -354,6 +377,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -937,15 +972,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:E28"/>
+  <dimension ref="A2:J37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.21"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="39.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.84"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1041,150 +1080,245 @@
         <v>60</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="14" t="n">
+        <v>1546387200000</v>
+      </c>
+      <c r="J11" s="15" t="n">
+        <f aca="false">I11/1000/(60*60*24) + 25569</f>
+        <v>43467</v>
+      </c>
+    </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14" t="s">
-        <v>35</v>
+      <c r="A12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="16" t="n">
+        <v>43467</v>
+      </c>
+      <c r="C12" s="16" t="n">
+        <v>43485</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <f aca="false">(C12-B12)+1</f>
+        <v>19</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="14" t="n">
+        <f aca="false">(B12 - DATEVALUE("1/1/1970"))*86400</f>
+        <v>1546387200</v>
+      </c>
+      <c r="C13" s="14" t="n">
+        <f aca="false">(C12 - DATEVALUE("1/1/1970"))*86400</f>
+        <v>1547942400</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <f aca="false">C13-B13</f>
+        <v>1555200</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <f aca="false">D13/B14</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <f aca="false">24*60*60</f>
+        <v>86400</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H15" s="16" t="n">
+        <v>43467</v>
+      </c>
+      <c r="I15" s="14" t="n">
+        <f aca="false">(H15 - DATEVALUE("1/1/1970"))*86400</f>
+        <v>1546387200</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B17" s="0" t="n">
         <f aca="false">C6/D3</f>
         <v>5</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="0" t="n">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="0" t="n">
         <f aca="false">E6/D3</f>
         <v>3</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="0" t="s">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="17"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="C17" s="0" t="n">
-        <f aca="false">C3-(B17/B13)</f>
-        <v>46</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <f aca="false">$C$3-((B17-$C$9)/$B$14)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>9</v>
+      <c r="D20" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <f aca="false">C3-(B21/B17)</f>
+        <v>46</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <f aca="false">$C$3-((B21-$C$9)/$B$18)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <f aca="false">600/12</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C21" s="0" t="n">
-        <f aca="false">E6/B21</f>
+      <c r="C25" s="0" t="n">
+        <f aca="false">E6/B25</f>
         <v>30</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B24" s="0" t="n">
-        <f aca="false">$C$9+A24*$C$21</f>
-        <v>20</v>
-      </c>
-      <c r="C24" s="0" t="n">
-        <f aca="false">$C$3-((B24-$C$9)/$B$14)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B25" s="0" t="n">
-        <f aca="false">$C$9+A25*$C$21</f>
-        <v>50</v>
-      </c>
-      <c r="C25" s="0" t="n">
-        <f aca="false">$C$3-((B25-$C$9)/$B$14)</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B26" s="0" t="n">
-        <f aca="false">$C$9+A26*$C$21</f>
-        <v>80</v>
-      </c>
-      <c r="C26" s="0" t="n">
-        <f aca="false">$C$3-((B26-$C$9)/$B$14)</f>
-        <v>30</v>
-      </c>
-    </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B27" s="0" t="n">
-        <f aca="false">$C$9+A27*$C$21</f>
-        <v>110</v>
-      </c>
-      <c r="C27" s="0" t="n">
-        <f aca="false">$C$3-((B27-$C$9)/$B$14)</f>
-        <v>20</v>
+      <c r="B27" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <f aca="false">$C$9+A28*$C$25</f>
+        <v>20</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <f aca="false">$C$3-((B28-$C$9)/$B$18)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <f aca="false">$C$9+A29*$C$25</f>
+        <v>50</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <f aca="false">$C$3-((B29-$C$9)/$B$18)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <f aca="false">$C$9+A30*$C$25</f>
+        <v>80</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <f aca="false">$C$3-((B30-$C$9)/$B$18)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <f aca="false">$C$9+A31*$C$25</f>
+        <v>110</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <f aca="false">$C$3-((B31-$C$9)/$B$18)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B28" s="0" t="n">
-        <f aca="false">$C$9+A28*$C$21</f>
+      <c r="B32" s="0" t="n">
+        <f aca="false">$C$9+A32*$C$25</f>
         <v>140</v>
       </c>
-      <c r="C28" s="0" t="n">
-        <f aca="false">$C$3-((B28-$C$9)/$B$14)</f>
+      <c r="C32" s="0" t="n">
+        <f aca="false">$C$3-((B32-$C$9)/$B$18)</f>
         <v>10</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <f aca="false">B6/D12</f>
+        <v>31.5789473684211</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>